<commit_message>
add logic to the stay button (1)
</commit_message>
<xml_diff>
--- a/assets/product-backlog.xlsx
+++ b/assets/product-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\javascript_learning\assignments\Blackjack\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3314B5-E1CA-42FD-AD4C-00C695F1B88D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDE1088-8AA5-481D-B0F7-6CB2E43D7B8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12920" xr2:uid="{273E3F6B-73CE-49FA-9A48-88CFBA41EF6F}"/>
   </bookViews>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>priority</t>
-  </si>
-  <si>
     <t>story points</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>I can get twice as much as the default profit</t>
   </si>
   <si>
-    <t>be able to look at the dealer's cards</t>
-  </si>
-  <si>
     <t>I can prove that the dealer is honest</t>
   </si>
   <si>
@@ -135,10 +129,19 @@
     <t>BJ-010</t>
   </si>
   <si>
-    <t xml:space="preserve">see the dealer's score </t>
-  </si>
-  <si>
     <t>see my current score, total number of remaining cards in the deck, as well as  my current money</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>see the other player's status (score etc. as same as BJ-009)</t>
+  </si>
+  <si>
+    <t>be able to look at the other player's cards</t>
   </si>
 </sst>
 </file>
@@ -530,7 +533,7 @@
   <dimension ref="A2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -545,161 +548,173 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -708,16 +723,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>

</xml_diff>

<commit_message>
add the register form (1)
</commit_message>
<xml_diff>
--- a/assets/product-backlog.xlsx
+++ b/assets/product-backlog.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\javascript_learning\assignments\Blackjack\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDE1088-8AA5-481D-B0F7-6CB2E43D7B8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849BD5F4-8D70-47E2-95D9-74A83EECC6D7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12920" xr2:uid="{273E3F6B-73CE-49FA-9A48-88CFBA41EF6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -75,9 +76,6 @@
     <t>User</t>
   </si>
   <si>
-    <t>bet on my game</t>
-  </si>
-  <si>
     <t>be able to hold my played cards</t>
   </si>
   <si>
@@ -90,9 +88,6 @@
     <t xml:space="preserve">I can validate my score </t>
   </si>
   <si>
-    <t>I can get more money from playing</t>
-  </si>
-  <si>
     <t>be able to hold my current condition at any turns</t>
   </si>
   <si>
@@ -111,9 +106,6 @@
     <t>I can get twice as much as the default profit</t>
   </si>
   <si>
-    <t>I can prove that the dealer is honest</t>
-  </si>
-  <si>
     <t>be able to input my full name and the amount of betting money</t>
   </si>
   <si>
@@ -124,9 +116,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>BJ-010</t>
   </si>
   <si>
     <t>see my current score, total number of remaining cards in the deck, as well as  my current money</t>
@@ -530,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F7B2D5A-6668-4ED3-8540-B4704BDBA106}">
-  <dimension ref="A2:F12"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -543,29 +532,47 @@
     <col min="5" max="5" width="10.3515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -574,16 +581,18 @@
         <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -592,150 +601,143 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11C5468-7BAA-42A9-A756-1DC8B7CFAA81}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="6.05859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.41015625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.87890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.234375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="E4" s="1">
-        <v>2</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1">
-        <v>5</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="1">
-        <v>3</v>
-      </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modify the UI for the game
</commit_message>
<xml_diff>
--- a/assets/product-backlog.xlsx
+++ b/assets/product-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\javascript_learning\assignments\Blackjack\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849BD5F4-8D70-47E2-95D9-74A83EECC6D7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A344233-8914-49EF-9FA6-B9CC3FA9A8A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12920" xr2:uid="{273E3F6B-73CE-49FA-9A48-88CFBA41EF6F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -131,6 +131,18 @@
   </si>
   <si>
     <t>be able to look at the other player's cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User  </t>
+  </si>
+  <si>
+    <t>be able to choose a desired score for a specific game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">be able to look at the game author's social media accounts </t>
+  </si>
+  <si>
+    <t>I can get some updates about author's another launched games</t>
   </si>
 </sst>
 </file>
@@ -174,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -197,14 +209,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,16 +543,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F7B2D5A-6668-4ED3-8540-B4704BDBA106}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="3" max="3" width="76.87890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.9375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.3515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -568,7 +592,9 @@
       <c r="E2" s="1">
         <v>3</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
@@ -608,6 +634,43 @@
       </c>
       <c r="F4" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -620,7 +683,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A5" sqref="A5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
modified the Social media button (from BJ005)
</commit_message>
<xml_diff>
--- a/assets/product-backlog.xlsx
+++ b/assets/product-backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IT\javascript_learning\assignments\Blackjack\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A344233-8914-49EF-9FA6-B9CC3FA9A8A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343CBD3E-028F-40B9-B79C-1AB17B9CD63C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12920" xr2:uid="{273E3F6B-73CE-49FA-9A48-88CFBA41EF6F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -543,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F7B2D5A-6668-4ED3-8540-B4704BDBA106}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -672,6 +672,25 @@
       <c r="E6" s="3">
         <v>1</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -683,7 +702,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F6"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -714,22 +733,6 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>10</v>

</xml_diff>